<commit_message>
update fig1 source data after ITA home isolation policy update
</commit_message>
<xml_diff>
--- a/results/source_data/fig1_source_data.xlsx
+++ b/results/source_data/fig1_source_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahking/gpl-covid/results/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF9F940-E4E1-0546-9052-216477A7BAC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3C7ED5-981B-C045-AE9C-750899F984C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3440" yWindow="1520" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3440" yWindow="1520" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fig1_epi_timeseries" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2785" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2784" uniqueCount="558">
   <si>
     <t>date</t>
   </si>
@@ -6392,8 +6392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G263"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="F259" sqref="F259"/>
+    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="I155" sqref="I155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6840,7 +6840,7 @@
         <v>43911</v>
       </c>
       <c r="B20">
-        <v>0.83000000000000196</v>
+        <v>0.83</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -6863,7 +6863,7 @@
         <v>43912</v>
       </c>
       <c r="B21">
-        <v>0.82999999999999796</v>
+        <v>0.83</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -6932,7 +6932,7 @@
         <v>43915</v>
       </c>
       <c r="B24">
-        <v>2.4550000000000098</v>
+        <v>2.4550000000000001</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -6941,7 +6941,7 @@
         <v>3.12</v>
       </c>
       <c r="E24">
-        <v>0.14000000000000101</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F24">
         <v>2.64</v>
@@ -6955,7 +6955,7 @@
         <v>43916</v>
       </c>
       <c r="B25">
-        <v>0.32999999999999802</v>
+        <v>0.33</v>
       </c>
       <c r="C25">
         <v>1.5</v>
@@ -6987,10 +6987,10 @@
         <v>1.6</v>
       </c>
       <c r="E26">
-        <v>0.32999999999999802</v>
+        <v>0.33</v>
       </c>
       <c r="F26">
-        <v>0.510000000000005</v>
+        <v>0.51</v>
       </c>
       <c r="G26" t="s">
         <v>4</v>
@@ -7007,10 +7007,10 @@
         <v>3</v>
       </c>
       <c r="D27">
-        <v>0.79999999999999705</v>
+        <v>0.8</v>
       </c>
       <c r="E27">
-        <v>0.149999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="F27">
         <v>1.57</v>
@@ -7030,13 +7030,13 @@
         <v>1.5</v>
       </c>
       <c r="D28">
-        <v>0.24000000000000199</v>
+        <v>0.24</v>
       </c>
       <c r="E28">
-        <v>0.14000000000000101</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F28">
-        <v>0.13999999999999299</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G28" t="s">
         <v>4</v>
@@ -7056,7 +7056,7 @@
         <v>2.09</v>
       </c>
       <c r="E29">
-        <v>0.14000000000000101</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F29">
         <v>1.1399999999999999</v>
@@ -7079,7 +7079,7 @@
         <v>0.5</v>
       </c>
       <c r="E30">
-        <v>0.149999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="F30">
         <v>1.1599999999999999</v>
@@ -7099,13 +7099,13 @@
         <v>2</v>
       </c>
       <c r="D31">
-        <v>0.84999999999999398</v>
+        <v>0.85</v>
       </c>
       <c r="E31">
-        <v>0.14000000000000101</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F31">
-        <v>0.96999999999999897</v>
+        <v>0.97</v>
       </c>
       <c r="G31" t="s">
         <v>4</v>
@@ -7220,7 +7220,7 @@
         <v>5</v>
       </c>
       <c r="F36">
-        <v>0.99000000000000199</v>
+        <v>0.99</v>
       </c>
       <c r="G36" t="s">
         <v>4</v>
@@ -8246,7 +8246,7 @@
         <v>5</v>
       </c>
       <c r="C81">
-        <v>10.40000013</v>
+        <v>10.4000001</v>
       </c>
       <c r="D81" t="s">
         <v>5</v>
@@ -8338,7 +8338,7 @@
         <v>5</v>
       </c>
       <c r="C85">
-        <v>0.19999998999999799</v>
+        <v>0.19999998999999999</v>
       </c>
       <c r="D85" t="s">
         <v>5</v>
@@ -9885,7 +9885,7 @@
         <v>11</v>
       </c>
       <c r="E152">
-        <v>35.31</v>
+        <v>7.59</v>
       </c>
       <c r="F152">
         <v>107</v>
@@ -9930,8 +9930,8 @@
       <c r="D154">
         <v>41.5</v>
       </c>
-      <c r="E154" t="s">
-        <v>5</v>
+      <c r="E154">
+        <v>27.72</v>
       </c>
       <c r="F154" t="s">
         <v>5</v>
@@ -10207,7 +10207,7 @@
         <v>53.5</v>
       </c>
       <c r="E166">
-        <v>3.9600000000000102</v>
+        <v>3.96</v>
       </c>
       <c r="F166" t="s">
         <v>5</v>
@@ -12456,7 +12456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F530"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>

</xml_diff>